<commit_message>
fix name not exist
</commit_message>
<xml_diff>
--- a/tools/relation.xlsx
+++ b/tools/relation.xlsx
@@ -137,7 +137,7 @@
         <sz val="12.0"/>
         <color rgb="FF000000"/>
       </rPr>
-      <t xml:space="preserve">劳拉·亚尔赛德</t>
+      <t xml:space="preserve">劳拉·S·亚尔赛德</t>
     </r>
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>
@@ -2270,7 +2270,7 @@
         <sz val="10.0"/>
         <color rgb="FF000000"/>
       </rPr>
-      <t xml:space="preserve">劳拉·亚尔赛德</t>
+      <t xml:space="preserve">劳拉·S·亚尔赛德</t>
     </r>
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>

</xml_diff>

<commit_message>
update parsing wiki page
</commit_message>
<xml_diff>
--- a/tools/relation.xlsx
+++ b/tools/relation.xlsx
@@ -1076,7 +1076,14 @@
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>
   <si>
-    <t xml:space="preserve">沃雷斯·拜尔迪安斯</t>
+    <r>
+      <rPr>
+        <rFont val="Microsoft YaHei"/>
+        <sz val="12.0"/>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t xml:space="preserve">渥雷斯·拜尔迪安斯</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>
   <si>
@@ -2681,7 +2688,7 @@
         <sz val="10.0"/>
         <color rgb="FF000000"/>
       </rPr>
-      <t xml:space="preserve">沃雷斯·拜尔迪安斯</t>
+      <t xml:space="preserve">渥雷斯·拜尔迪安斯</t>
     </r>
     <phoneticPr fontId="1" type="noConversion" alignment="left"/>
   </si>

</xml_diff>